<commit_message>
feat: refactor config, support plasmid features
This commit adds the ability to specify features (specifically,
resistance genes and origins of replication) for plasmids.  While making
this change, I realized that the options read from the config file
should be stored in the database object, and not in a global variable.
I fixed this as well, and while I was at it I made the config file
system more flexibile in terms of file/directory layout and reagent
naming conventions (both things I'd been meaning to do for a while).

Fixes #10
Fixes #12
</commit_message>
<xml_diff>
--- a/tests/mock_excel_db/buffers.xlsx
+++ b/tests/mock_excel_db/buffers.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t xml:space="preserve">Name</t>
+    <t xml:space="preserve">Tag</t>
   </si>
   <si>
     <t xml:space="preserve">b2</t>
@@ -100,8 +100,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -127,18 +131,18 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: refactor config, support plasmid features (#22)
* feat: refactor config, support plasmid features

This commit adds the ability to specify features (specifically,
resistance genes and origins of replication) for plasmids.  While making
this change, I realized that the options read from the config file
should be stored in the database object, and not in a global variable.
I fixed this as well, and while I was at it I made the config file
system more flexibile in terms of file/directory layout and reagent
naming conventions (both things I'd been meaning to do for a while).

Fixes #10
Fixes #12

* chore: add rtoml dependency

* chore: run tests for python 3.10

* chore: don't support python 3.10 yet

rtoml doesn't have wheels for python 3.10 yet, so it's hard to install on CI.
</commit_message>
<xml_diff>
--- a/tests/mock_excel_db/buffers.xlsx
+++ b/tests/mock_excel_db/buffers.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t xml:space="preserve">Name</t>
+    <t xml:space="preserve">Tag</t>
   </si>
   <si>
     <t xml:space="preserve">b2</t>
@@ -100,8 +100,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -127,18 +131,18 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>